<commit_message>
modify frm_match_100 with a list of WebBrowser
modify frm_match_100 with a list of WebBrowser
add Extension.CS
</commit_message>
<xml_diff>
--- a/web_helper/data/DataTable.xlsx
+++ b/web_helper/data/DataTable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="124">
   <si>
     <t>timespan</t>
   </si>
@@ -1938,7 +1938,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1974,6 +1974,11 @@
         <v>118</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
modify table name and update frm_match_100
modify table name and update frm_match_100
</commit_message>
<xml_diff>
--- a/web_helper/data/DataTable.xlsx
+++ b/web_helper/data/DataTable.xlsx
@@ -4,22 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
     <sheet name="mix_match" sheetId="2" r:id="rId2"/>
     <sheet name="compute method" sheetId="3" r:id="rId3"/>
-    <sheet name="europe" sheetId="4" r:id="rId4"/>
-    <sheet name="europe_new" sheetId="6" r:id="rId5"/>
+    <sheet name="europe_500_log" sheetId="4" r:id="rId4"/>
+    <sheet name="europe_500" sheetId="6" r:id="rId5"/>
     <sheet name="doc_info" sheetId="7" r:id="rId6"/>
+    <sheet name="europe_100_log" sheetId="8" r:id="rId7"/>
+    <sheet name="europe_100" sheetId="9" r:id="rId8"/>
+    <sheet name="company" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="124">
   <si>
     <t>timespan</t>
   </si>
@@ -893,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1385,7 +1388,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1459,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1699,7 +1702,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1935,10 +1938,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1974,43 +1977,536 @@
         <v>118</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new table team and modify dome bug
modify frm_match_500_team
add new table team
add two function get_24h(),get_12m() to Match100Helper class
</commit_message>
<xml_diff>
--- a/web_helper/data/DataTable.xlsx
+++ b/web_helper/data/DataTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="europe_100" sheetId="9" r:id="rId8"/>
     <sheet name="company" sheetId="10" r:id="rId9"/>
     <sheet name="company_url" sheetId="11" r:id="rId10"/>
+    <sheet name="teams" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="141">
   <si>
     <t>timespan</t>
   </si>
@@ -415,6 +416,42 @@
   </si>
   <si>
     <t>seconds</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>select_type</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>nvarchar(500)</t>
+  </si>
+  <si>
+    <t>nvarchar(4000)</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name2 </t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>english name</t>
+  </si>
+  <si>
+    <t>chinese name</t>
+  </si>
+  <si>
+    <t>cantonese name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id </t>
   </si>
 </sst>
 </file>
@@ -910,10 +947,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -921,39 +958,137 @@
     <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>126</v>
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2010,7 +2145,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F18"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2055,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2531,10 +2666,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2542,44 +2677,65 @@
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new table match_future
add new table match_future
add function to get future match information
</commit_message>
<xml_diff>
--- a/web_helper/data/DataTable.xlsx
+++ b/web_helper/data/DataTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="722" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="single" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="company" sheetId="10" r:id="rId9"/>
     <sheet name="company_url" sheetId="11" r:id="rId10"/>
     <sheet name="teams" sheetId="12" r:id="rId11"/>
+    <sheet name="future_match" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="141">
   <si>
     <t>timespan</t>
   </si>
@@ -1031,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1089,6 +1090,65 @@
       </c>
       <c r="B5" t="s">
         <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>